<commit_message>
updated data flow to sql db and some minor updates
</commit_message>
<xml_diff>
--- a/coins.xlsx
+++ b/coins.xlsx
@@ -15,240 +15,339 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>Date/Coins</t>
   </si>
   <si>
+    <t>DENTBTC</t>
+  </si>
+  <si>
+    <t>STEEMBTC</t>
+  </si>
+  <si>
+    <t>POWRBTC</t>
+  </si>
+  <si>
+    <t>VIBBTC</t>
+  </si>
+  <si>
+    <t>INSBTC</t>
+  </si>
+  <si>
+    <t>BNBBTC</t>
+  </si>
+  <si>
+    <t>AMBBTC</t>
+  </si>
+  <si>
+    <t>TUSDBTC</t>
+  </si>
+  <si>
+    <t>IOTABTC</t>
+  </si>
+  <si>
+    <t>ICXBTC</t>
+  </si>
+  <si>
+    <t>BLZBTC</t>
+  </si>
+  <si>
+    <t>SALTBTC</t>
+  </si>
+  <si>
+    <t>XEMBTC</t>
+  </si>
+  <si>
+    <t>ADABTC</t>
+  </si>
+  <si>
+    <t>THETABTC</t>
+  </si>
+  <si>
+    <t>BNTBTC</t>
+  </si>
+  <si>
+    <t>XLMBTC</t>
+  </si>
+  <si>
     <t>ETHBTC</t>
   </si>
   <si>
-    <t>BNBBTC</t>
+    <t>NULSBTC</t>
+  </si>
+  <si>
+    <t>LRCBTC</t>
+  </si>
+  <si>
+    <t>QSPBTC</t>
+  </si>
+  <si>
+    <t>WINGSBTC</t>
+  </si>
+  <si>
+    <t>GNTBTC</t>
+  </si>
+  <si>
+    <t>AIONBTC</t>
+  </si>
+  <si>
+    <t>GTOBTC</t>
+  </si>
+  <si>
+    <t>ARDRBTC</t>
+  </si>
+  <si>
+    <t>OMGBTC</t>
+  </si>
+  <si>
+    <t>REQBTC</t>
+  </si>
+  <si>
+    <t>STORJBTC</t>
+  </si>
+  <si>
+    <t>XVGBTC</t>
+  </si>
+  <si>
+    <t>DGDBTC</t>
+  </si>
+  <si>
+    <t>ZILBTC</t>
+  </si>
+  <si>
+    <t>TNBBTC</t>
+  </si>
+  <si>
+    <t>BTSBTC</t>
+  </si>
+  <si>
+    <t>LTCBTC</t>
+  </si>
+  <si>
+    <t>EVXBTC</t>
+  </si>
+  <si>
+    <t>IOSTBTC</t>
   </si>
   <si>
     <t>BCCBTC</t>
   </si>
   <si>
+    <t>CNDBTC</t>
+  </si>
+  <si>
+    <t>OAXBTC</t>
+  </si>
+  <si>
+    <t>NEOBTC</t>
+  </si>
+  <si>
+    <t>PAXBTC</t>
+  </si>
+  <si>
+    <t>HOTBTC</t>
+  </si>
+  <si>
+    <t>BTGBTC</t>
+  </si>
+  <si>
+    <t>DASHBTC</t>
+  </si>
+  <si>
+    <t>BCDBTC</t>
+  </si>
+  <si>
+    <t>BTCUSDT</t>
+  </si>
+  <si>
+    <t>ADXBTC</t>
+  </si>
+  <si>
+    <t>LUNBTC</t>
+  </si>
+  <si>
+    <t>BRDBTC</t>
+  </si>
+  <si>
+    <t>BCPTBTC</t>
+  </si>
+  <si>
+    <t>NEBLBTC</t>
+  </si>
+  <si>
+    <t>XRPBTC</t>
+  </si>
+  <si>
+    <t>RDNBTC</t>
+  </si>
+  <si>
+    <t>EOSBTC</t>
+  </si>
+  <si>
+    <t>ENJBTC</t>
+  </si>
+  <si>
+    <t>SNTBTC</t>
+  </si>
+  <si>
+    <t>TRXBTC</t>
+  </si>
+  <si>
+    <t>QTUMBTC</t>
+  </si>
+  <si>
+    <t>SYSBTC</t>
+  </si>
+  <si>
+    <t>XMRBTC</t>
+  </si>
+  <si>
+    <t>ZRXBTC</t>
+  </si>
+  <si>
+    <t>NCASHBTC</t>
+  </si>
+  <si>
+    <t>GASBTC</t>
+  </si>
+  <si>
+    <t>FUNBTC</t>
+  </si>
+  <si>
+    <t>SUBBTC</t>
+  </si>
+  <si>
     <t>MCOBTC</t>
   </si>
   <si>
-    <t>LRCBTC</t>
-  </si>
-  <si>
-    <t>QTUMBTC</t>
-  </si>
-  <si>
-    <t>OMGBTC</t>
+    <t>SNGLSBTC</t>
+  </si>
+  <si>
+    <t>MANABTC</t>
+  </si>
+  <si>
+    <t>ASTBTC</t>
   </si>
   <si>
     <t>STRATBTC</t>
   </si>
   <si>
+    <t>NPXSBTC</t>
+  </si>
+  <si>
+    <t>ZECBTC</t>
+  </si>
+  <si>
     <t>BQXBTC</t>
   </si>
   <si>
-    <t>FUNBTC</t>
-  </si>
-  <si>
-    <t>IOTABTC</t>
-  </si>
-  <si>
-    <t>SALTBTC</t>
-  </si>
-  <si>
-    <t>EOSBTC</t>
-  </si>
-  <si>
-    <t>SNTBTC</t>
+    <t>ELFBTC</t>
+  </si>
+  <si>
+    <t>ZENBTC</t>
+  </si>
+  <si>
+    <t>ENGBTC</t>
   </si>
   <si>
     <t>MTHBTC</t>
   </si>
   <si>
-    <t>ENGBTC</t>
-  </si>
-  <si>
-    <t>ZECBTC</t>
-  </si>
-  <si>
-    <t>BNTBTC</t>
-  </si>
-  <si>
-    <t>ASTBTC</t>
-  </si>
-  <si>
-    <t>DASHBTC</t>
-  </si>
-  <si>
-    <t>OAXBTC</t>
-  </si>
-  <si>
-    <t>BTGBTC</t>
-  </si>
-  <si>
-    <t>EVXBTC</t>
-  </si>
-  <si>
-    <t>REQBTC</t>
-  </si>
-  <si>
-    <t>VIBBTC</t>
-  </si>
-  <si>
-    <t>TRXBTC</t>
-  </si>
-  <si>
-    <t>POWRBTC</t>
+    <t>AEBTC</t>
+  </si>
+  <si>
+    <t>WANBTC</t>
+  </si>
+  <si>
+    <t>HCBTC</t>
+  </si>
+  <si>
+    <t>PIVXBTC</t>
+  </si>
+  <si>
+    <t>QLCBTC</t>
+  </si>
+  <si>
+    <t>KMDBTC</t>
+  </si>
+  <si>
+    <t>POEBTC</t>
+  </si>
+  <si>
+    <t>POABTC</t>
+  </si>
+  <si>
+    <t>NANOBTC</t>
+  </si>
+  <si>
+    <t>GXSBTC</t>
+  </si>
+  <si>
+    <t>KEYBTC</t>
+  </si>
+  <si>
+    <t>CLOAKBTC</t>
   </si>
   <si>
     <t>ARKBTC</t>
   </si>
   <si>
-    <t>XRPBTC</t>
-  </si>
-  <si>
-    <t>ENJBTC</t>
-  </si>
-  <si>
-    <t>STORJBTC</t>
-  </si>
-  <si>
-    <t>NULSBTC</t>
-  </si>
-  <si>
-    <t>RDNBTC</t>
-  </si>
-  <si>
-    <t>XMRBTC</t>
-  </si>
-  <si>
-    <t>AMBBTC</t>
-  </si>
-  <si>
-    <t>BATBTC</t>
-  </si>
-  <si>
-    <t>BCPTBTC</t>
+    <t>DLTBTC</t>
+  </si>
+  <si>
+    <t>POLYBTC</t>
+  </si>
+  <si>
+    <t>RLCBTC</t>
+  </si>
+  <si>
+    <t>KNCBTC</t>
   </si>
   <si>
     <t>ARNBTC</t>
   </si>
   <si>
-    <t>GVTBTC</t>
-  </si>
-  <si>
-    <t>QSPBTC</t>
-  </si>
-  <si>
-    <t>TNTBTC</t>
-  </si>
-  <si>
-    <t>BCDBTC</t>
-  </si>
-  <si>
-    <t>ADXBTC</t>
-  </si>
-  <si>
-    <t>PPTBTC</t>
-  </si>
-  <si>
-    <t>XLMBTC</t>
-  </si>
-  <si>
-    <t>GTOBTC</t>
-  </si>
-  <si>
-    <t>ICXBTC</t>
-  </si>
-  <si>
-    <t>AIONBTC</t>
-  </si>
-  <si>
-    <t>BRDBTC</t>
-  </si>
-  <si>
-    <t>WINGSBTC</t>
-  </si>
-  <si>
-    <t>NAVBTC</t>
-  </si>
-  <si>
-    <t>LUNBTC</t>
-  </si>
-  <si>
-    <t>APPCBTC</t>
+    <t>NXSBTC</t>
   </si>
   <si>
     <t>VIBEBTC</t>
   </si>
   <si>
-    <t>INSBTC</t>
-  </si>
-  <si>
-    <t>IOSTBTC</t>
-  </si>
-  <si>
-    <t>NANOBTC</t>
-  </si>
-  <si>
-    <t>BLZBTC</t>
-  </si>
-  <si>
-    <t>NCASHBTC</t>
-  </si>
-  <si>
-    <t>POABTC</t>
-  </si>
-  <si>
-    <t>ZILBTC</t>
-  </si>
-  <si>
-    <t>ONTBTC</t>
-  </si>
-  <si>
-    <t>QLCBTC</t>
-  </si>
-  <si>
-    <t>SYSBTC</t>
-  </si>
-  <si>
-    <t>CLOAKBTC</t>
-  </si>
-  <si>
-    <t>GNTBTC</t>
-  </si>
-  <si>
-    <t>LOOMBTC</t>
-  </si>
-  <si>
-    <t>TUSDBTC</t>
-  </si>
-  <si>
-    <t>ZENBTC</t>
-  </si>
-  <si>
-    <t>NPXSBTC</t>
-  </si>
-  <si>
-    <t>NASBTC</t>
-  </si>
-  <si>
-    <t>DENTBTC</t>
-  </si>
-  <si>
-    <t>ARDRBTC</t>
-  </si>
-  <si>
-    <t>HOTBTC</t>
-  </si>
-  <si>
-    <t>POLYBTC</t>
-  </si>
-  <si>
-    <t>HCBTC</t>
-  </si>
-  <si>
-    <t>PAXBTC</t>
+    <t>VIABTC</t>
+  </si>
+  <si>
+    <t>MDABTC</t>
+  </si>
+  <si>
+    <t>MODBTC</t>
+  </si>
+  <si>
+    <t>XZCBTC</t>
+  </si>
+  <si>
+    <t>SKYBTC</t>
+  </si>
+  <si>
+    <t>DATABTC</t>
+  </si>
+  <si>
+    <t>LSKBTC</t>
+  </si>
+  <si>
+    <t>AGIBTC</t>
+  </si>
+  <si>
+    <t>ETCBTC</t>
+  </si>
+  <si>
+    <t>SNMBTC</t>
+  </si>
+  <si>
+    <t>OSTBTC</t>
+  </si>
+  <si>
+    <t>EDOBTC</t>
   </si>
 </sst>
 </file>
@@ -587,7 +686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BZ2"/>
+  <dimension ref="A1:DG11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,7 +694,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:78">
+    <row r="1" spans="1:111">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -830,241 +929,1093 @@
       <c r="BZ1" t="s">
         <v>77</v>
       </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>105</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="2" spans="1:78">
+    <row r="2" spans="1:111">
       <c r="A2" s="1" t="n">
-        <v>43405.96055006304</v>
+        <v>43407.01803385979</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0311585</v>
+        <v>4.25e-07</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00149895</v>
+        <v>0.00012585</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06674849999999999</v>
+        <v>2.559e-05</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0006945</v>
+        <v>8.165000000000001e-06</v>
       </c>
       <c r="F2" t="n">
-        <v>1.875e-05</v>
+        <v>7.439999999999999e-05</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0006065000000000001</v>
+        <v>0.00149855</v>
       </c>
       <c r="H2" t="n">
-        <v>0.000514</v>
+        <v>2.919e-05</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0002453</v>
+        <v>0.00015682</v>
       </c>
       <c r="J2" t="n">
-        <v>6.2185e-05</v>
+        <v>7.577e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>2.22e-06</v>
+        <v>0.00010005</v>
       </c>
       <c r="L2" t="n">
-        <v>7.414499999999999e-05</v>
+        <v>2.355e-05</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0001077</v>
+        <v>0.0001143</v>
       </c>
       <c r="N2" t="n">
-        <v>0.00082315</v>
+        <v>1.474e-05</v>
       </c>
       <c r="O2" t="n">
-        <v>6.195e-06</v>
+        <v>1.1355e-05</v>
       </c>
       <c r="P2" t="n">
-        <v>6.58e-06</v>
+        <v>1.467e-05</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.000104</v>
+        <v>0.00021061</v>
       </c>
       <c r="R2" t="n">
-        <v>0.018178</v>
+        <v>3.63e-05</v>
       </c>
       <c r="S2" t="n">
-        <v>0.00020836</v>
+        <v>0.031497</v>
       </c>
       <c r="T2" t="n">
-        <v>1.571e-05</v>
+        <v>0.000176855</v>
       </c>
       <c r="U2" t="n">
-        <v>0.024086</v>
+        <v>1.8295e-05</v>
       </c>
       <c r="V2" t="n">
-        <v>4.0985e-05</v>
+        <v>7.005e-06</v>
       </c>
       <c r="W2" t="n">
-        <v>0.004184</v>
+        <v>2.801e-05</v>
       </c>
       <c r="X2" t="n">
-        <v>8.3605e-05</v>
+        <v>2.705e-05</v>
       </c>
       <c r="Y2" t="n">
-        <v>8.415e-06</v>
+        <v>6.655e-05</v>
       </c>
       <c r="Z2" t="n">
-        <v>8.194999999999999e-06</v>
+        <v>1.064e-05</v>
       </c>
       <c r="AA2" t="n">
-        <v>3.5e-06</v>
+        <v>1.713e-05</v>
       </c>
       <c r="AB2" t="n">
-        <v>2.5945e-05</v>
+        <v>0.0005074999999999999</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.0001266</v>
+        <v>8.33e-06</v>
       </c>
       <c r="AD2" t="n">
-        <v>7.170000000000001e-05</v>
+        <v>5.193e-05</v>
       </c>
       <c r="AE2" t="n">
-        <v>8.015e-06</v>
+        <v>2.165e-06</v>
       </c>
       <c r="AF2" t="n">
-        <v>5.341000000000001e-05</v>
+        <v>0.00646</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.000181605</v>
+        <v>5.605e-06</v>
       </c>
       <c r="AH2" t="n">
-        <v>8.848499999999999e-05</v>
+        <v>1.75e-06</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.016261</v>
+        <v>1.5065e-05</v>
       </c>
       <c r="AJ2" t="n">
-        <v>2.901e-05</v>
+        <v>0.00805</v>
       </c>
       <c r="AK2" t="n">
-        <v>4.0065e-05</v>
+        <v>8.400500000000001e-05</v>
       </c>
       <c r="AL2" t="n">
-        <v>1.821e-05</v>
+        <v>1.905e-06</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.00011199</v>
+        <v>0.072879</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.0018482</v>
+        <v>4.015e-06</v>
       </c>
       <c r="AO2" t="n">
-        <v>7.09e-06</v>
+        <v>4.092e-05</v>
       </c>
       <c r="AP2" t="n">
-        <v>5.539999999999999e-06</v>
+        <v>0.002525</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.000266</v>
+        <v>0.000156465</v>
       </c>
       <c r="AR2" t="n">
-        <v>3.7e-05</v>
+        <v>1.65e-07</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.00058095</v>
+        <v>0.004281500000000001</v>
       </c>
       <c r="AT2" t="n">
-        <v>3.526e-05</v>
+        <v>0.0242375</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.0825e-05</v>
+        <v>0.0002685</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.00010155</v>
+        <v>6431.9</v>
       </c>
       <c r="AW2" t="n">
-        <v>6.68e-05</v>
+        <v>3.623e-05</v>
       </c>
       <c r="AX2" t="n">
-        <v>5.664999999999999e-05</v>
+        <v>0.0007061</v>
       </c>
       <c r="AY2" t="n">
-        <v>2.805e-05</v>
+        <v>5.5535e-05</v>
       </c>
       <c r="AZ2" t="n">
-        <v>6.095e-05</v>
+        <v>1.843e-05</v>
       </c>
       <c r="BA2" t="n">
-        <v>0.00070545</v>
+        <v>0.0003885</v>
       </c>
       <c r="BB2" t="n">
-        <v>2.0855e-05</v>
+        <v>7.1975e-05</v>
       </c>
       <c r="BC2" t="n">
-        <v>1.103e-05</v>
+        <v>8.705e-05</v>
       </c>
       <c r="BD2" t="n">
-        <v>7.485e-05</v>
+        <v>0.0008388499999999999</v>
       </c>
       <c r="BE2" t="n">
-        <v>1.91e-06</v>
+        <v>7.845e-06</v>
       </c>
       <c r="BF2" t="n">
-        <v>0.00030715</v>
+        <v>6.075e-06</v>
       </c>
       <c r="BG2" t="n">
-        <v>2.224e-05</v>
+        <v>3.575e-06</v>
       </c>
       <c r="BH2" t="n">
-        <v>8.65e-07</v>
+        <v>0.0006165</v>
       </c>
       <c r="BI2" t="n">
-        <v>1.721e-05</v>
+        <v>1.4635e-05</v>
       </c>
       <c r="BJ2" t="n">
-        <v>5.62e-06</v>
+        <v>0.0165785</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.0002654</v>
+        <v>0.000127245</v>
       </c>
       <c r="BL2" t="n">
-        <v>8.369999999999999e-06</v>
+        <v>8.4e-07</v>
       </c>
       <c r="BM2" t="n">
-        <v>1.498e-05</v>
+        <v>0.0007975</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.0004542</v>
+        <v>2.185e-06</v>
       </c>
       <c r="BO2" t="n">
-        <v>2.695e-05</v>
+        <v>1.796e-05</v>
       </c>
       <c r="BP2" t="n">
-        <v>1.853e-05</v>
+        <v>0.0006865</v>
       </c>
       <c r="BQ2" t="n">
-        <v>0.000157505</v>
+        <v>4.725e-06</v>
       </c>
       <c r="BR2" t="n">
-        <v>0.0023</v>
+        <v>1.2515e-05</v>
       </c>
       <c r="BS2" t="n">
+        <v>1.639e-05</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>0.00025705</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>2.45e-07</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>0.0184025</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>6.0675e-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:111">
+      <c r="A3" s="1" t="n">
+        <v>43407.61611207916</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.000124</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.5235e-05</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.18e-06</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7.334999999999999e-05</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0014956</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.927e-05</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.00015788</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7.487999999999999e-05</v>
+      </c>
+      <c r="K3" t="n">
+        <v>9.905e-05</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0001159</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.461e-05</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1.122e-05</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.4385e-05</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.00020953</v>
+      </c>
+      <c r="R3" t="n">
+        <v>3.7295e-05</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.0313895</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.00017529</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1.8125e-05</v>
+      </c>
+      <c r="V3" t="n">
+        <v>7.01e-06</v>
+      </c>
+      <c r="W3" t="n">
+        <v>2.731e-05</v>
+      </c>
+      <c r="X3" t="n">
+        <v>2.6785e-05</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>1.0345e-05</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1.7525e-05</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.000504</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>8.040000000000001e-06</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>4.9865e-05</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0.006496</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>5.515e-06</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>1.72e-06</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.008028500000000001</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>8.332500000000001e-05</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>1.9e-06</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.0745555</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>3.97e-06</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.0025105</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.000157745</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1.7e-07</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.0242865</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>6360.690000000001</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>3.4975e-05</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0.0006735000000000001</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>7.173499999999999e-05</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>8.491e-05</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0.00084005</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>7.765000000000001e-06</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>6.079999999999999e-06</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>3.56e-06</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.0006075</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>1.4535e-05</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.016534</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.00012643</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>8.249999999999999e-07</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0.000795</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>2.17e-06</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>1.7665e-05</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0.0006985</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>4.645e-06</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>1.5545e-05</v>
+      </c>
+      <c r="BU3" t="n">
         <v>2.5e-07</v>
       </c>
-      <c r="BT2" t="n">
-        <v>0.0002351</v>
-      </c>
-      <c r="BU2" t="n">
-        <v>4.25e-07</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>1.71e-05</v>
-      </c>
-      <c r="BW2" t="n">
-        <v>1.65e-07</v>
-      </c>
-      <c r="BX2" t="n">
-        <v>4.599e-05</v>
-      </c>
-      <c r="BY2" t="n">
-        <v>0.0002919</v>
-      </c>
-      <c r="BZ2" t="n">
-        <v>0.00015749</v>
+      <c r="BV3" t="n">
+        <v>0.018366</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>5.9075e-05</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>4.9945e-05</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>0.002147</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>9.862e-05</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>6.75e-06</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>0.000188</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>0.000165</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>0.00029275</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>0.00021775</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>8.399999999999999e-06</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>0.00020025</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>2.11e-06</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>1.641e-05</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>0.0003042</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>0.00021275</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>1.2e-06</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>0.0004509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:111">
+      <c r="A4" s="1" t="n">
+        <v>43407.9876286462</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.00012415</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.5205e-05</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8.260000000000001e-06</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0014995</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.8655e-05</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.000157475</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7.47e-05</v>
+      </c>
+      <c r="K4" t="n">
+        <v>9.87e-05</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1.4655e-05</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1.124e-05</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.4405e-05</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.000209115</v>
+      </c>
+      <c r="R4" t="n">
+        <v>3.7495e-05</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.031366</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.000174415</v>
+      </c>
+      <c r="W4" t="n">
+        <v>2.751e-05</v>
+      </c>
+      <c r="X4" t="n">
+        <v>2.675e-05</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>1.0455e-05</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1.759e-05</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.0005020000000000001</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>7.995000000000001e-06</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>4.967e-05</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0.006507</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>5.485e-06</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>1.72e-06</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>1.506e-05</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.0080295</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>8.392e-05</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1.89e-06</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>4.005e-06</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.002507</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.000156955</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>1.7e-07</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.024402</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>6383.335</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>3.547499999999999e-05</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0.00067265</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>1.7935e-05</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>7.1665e-05</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>8.5005e-05</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>0.0008342</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>7.679999999999999e-06</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>5.99e-06</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>3.55e-06</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0.0006100000000000001</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>1.442e-05</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.016707</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>0.000125345</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>8.45e-07</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0.0007905</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>2.14e-06</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>1.7645e-05</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>0.000704</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>4.605e-06</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>1.5195e-05</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>0.00024895</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>2.4e-07</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>0.018353</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>5.9315e-05</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>0.002168</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>9.828e-05</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>6.78e-06</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>0.0001872</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>0.0002916</v>
+      </c>
+      <c r="CF4" t="n">
+        <v>8.364999999999999e-06</v>
+      </c>
+      <c r="CG4" t="n">
+        <v>0.00020055</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>1.6085e-05</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>0.0003031</v>
+      </c>
+      <c r="CL4" t="n">
+        <v>1.32e-06</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>0.00012525</v>
+      </c>
+      <c r="CO4" t="n">
+        <v>1.568e-05</v>
+      </c>
+      <c r="CP4" t="n">
+        <v>4.565e-05</v>
+      </c>
+      <c r="CQ4" t="n">
+        <v>7.035e-05</v>
+      </c>
+      <c r="CR4" t="n">
+        <v>6.5695e-05</v>
+      </c>
+      <c r="CS4" t="n">
+        <v>0.000111515</v>
+      </c>
+      <c r="CT4" t="n">
+        <v>0.0001068</v>
+      </c>
+      <c r="CU4" t="n">
+        <v>1.0495e-05</v>
+      </c>
+      <c r="CV4" t="n">
+        <v>0.0001208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:111">
+      <c r="A5" s="1" t="n">
+        <v>43408.02866793529</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8.245e-06</v>
+      </c>
+      <c r="X5" t="n">
+        <v>2.6755e-05</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>4.968e-05</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>3.5505e-05</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0.0006724000000000001</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>3.55e-06</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>8.45e-07</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0.00079</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>4.6e-06</v>
+      </c>
+      <c r="CL5" t="n">
+        <v>1.335e-06</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>6.562e-05</v>
+      </c>
+      <c r="CV5" t="n">
+        <v>0.000121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:111">
+      <c r="A6" s="1" t="n">
+        <v>43408.03062125808</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8.245e-06</v>
+      </c>
+      <c r="X6" t="n">
+        <v>2.6755e-05</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>4.9605e-05</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>3.542499999999999e-05</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.00067245</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>3.555e-06</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>8.5e-07</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0.00079</v>
+      </c>
+      <c r="CL6" t="n">
+        <v>1.33e-06</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>1.5645e-05</v>
+      </c>
+      <c r="CR6" t="n">
+        <v>6.562e-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:111">
+      <c r="A7" s="1" t="n">
+        <v>43408.03081046664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:111">
+      <c r="A8" s="1" t="n">
+        <v>43408.03134394315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:111">
+      <c r="A9" s="1" t="n">
+        <v>43415.75201202118</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>4.753e-05</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>3.3865e-05</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>3.565e-06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:111">
+      <c r="A10" s="1" t="n">
+        <v>43415.75490320772</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.00015844</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>4.7555e-05</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>3.3895e-05</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>5.468e-05</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>7.8705e-05</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>0.00083265</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>3.56e-06</v>
+      </c>
+      <c r="CF10" t="n">
+        <v>8.19e-06</v>
+      </c>
+      <c r="CN10" t="n">
+        <v>0.0001109</v>
+      </c>
+      <c r="CW10" t="n">
+        <v>0.00018016</v>
+      </c>
+      <c r="CX10" t="n">
+        <v>0.00012825</v>
+      </c>
+      <c r="CY10" t="n">
+        <v>0.0016555</v>
+      </c>
+    </row>
+    <row r="11" spans="1:111">
+      <c r="A11" s="1" t="n">
+        <v>43417.88146151772</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.00145115</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3.0075e-05</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.00015928</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7.646000000000001e-05</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.681e-05</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.162e-05</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1.3665e-05</v>
+      </c>
+      <c r="R11" t="n">
+        <v>4.0255e-05</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.032484</v>
+      </c>
+      <c r="W11" t="n">
+        <v>2.7125e-05</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.0005005000000000001</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>5.225e-06</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0.007813000000000001</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>1.81e-06</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>0.08182500000000001</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>4.2705e-05</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>0.0024105</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0.000158995</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.025159</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>6463.67</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>5.4565e-05</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>7.98e-05</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>0.0008172500000000001</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>7.794999999999999e-06</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>5.535e-06</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>3.465e-06</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>0.016389</v>
+      </c>
+      <c r="BO11" t="n">
+        <v>1.654e-05</v>
+      </c>
+      <c r="BU11" t="n">
+        <v>2.35e-07</v>
+      </c>
+      <c r="BV11" t="n">
+        <v>0.019976</v>
+      </c>
+      <c r="BZ11" t="n">
+        <v>9.062499999999999e-05</v>
+      </c>
+      <c r="CA11" t="n">
+        <v>7.47e-06</v>
+      </c>
+      <c r="CE11" t="n">
+        <v>0.00020645</v>
+      </c>
+      <c r="CF11" t="n">
+        <v>7.875e-06</v>
+      </c>
+      <c r="CH11" t="n">
+        <v>1.87e-06</v>
+      </c>
+      <c r="CK11" t="n">
+        <v>0.0001976</v>
+      </c>
+      <c r="CL11" t="n">
+        <v>1.04e-06</v>
+      </c>
+      <c r="CY11" t="n">
+        <v>0.0016145</v>
+      </c>
+      <c r="CZ11" t="n">
+        <v>0.000441</v>
+      </c>
+      <c r="DA11" t="n">
+        <v>6.145e-06</v>
+      </c>
+      <c r="DB11" t="n">
+        <v>0.0004026</v>
+      </c>
+      <c r="DC11" t="n">
+        <v>1.12e-05</v>
+      </c>
+      <c r="DD11" t="n">
+        <v>0.001416</v>
+      </c>
+      <c r="DE11" t="n">
+        <v>8.99e-06</v>
+      </c>
+      <c r="DF11" t="n">
+        <v>7.44e-06</v>
+      </c>
+      <c r="DG11" t="n">
+        <v>0.0002083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>